<commit_message>
Resolved Warnings and Messages
</commit_message>
<xml_diff>
--- a/Bug Report.xlsx
+++ b/Bug Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://w2shared-my.sharepoint.com/personal/dave_sushames01_student_wandw_ac_nz/Documents/Documents/Testing and Secure Coding/GroupAssignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="93" documentId="13_ncr:1_{D60B37C8-F51D-4837-A8FB-505AED30BC04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5E3C573-1B1B-4192-B4EA-F52361FA022A}"/>
+  <xr:revisionPtr revIDLastSave="115" documentId="13_ncr:1_{D60B37C8-F51D-4837-A8FB-505AED30BC04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6108400-6AEC-4969-837D-98142F126B56}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="165" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="98">
   <si>
     <t>Severity Legend</t>
   </si>
@@ -372,12 +372,42 @@
   <si>
     <t>Admin Sort ZA button</t>
   </si>
+  <si>
+    <t>004</t>
+  </si>
+  <si>
+    <t>"Invalid Email/Password" error changes</t>
+  </si>
+  <si>
+    <t>Error msg changes depending on if the entered password matches the criteria or not</t>
+  </si>
+  <si>
+    <t>1. Go to Login page 
+2. Enter Email
+3. Enter Incorrect password "123"
+4. Enter Incorrect password "Test@123"</t>
+  </si>
+  <si>
+    <t>Should always say "Invalid Email or Password"</t>
+  </si>
+  <si>
+    <t>Says "Password must be at least 8 characters long and contain upper, lower, number, and special character."</t>
+  </si>
+  <si>
+    <t>Sachith</t>
+  </si>
+  <si>
+    <t>Login password</t>
+  </si>
+  <si>
+    <t>TC_BBT_10</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -435,6 +465,12 @@
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -517,7 +553,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -585,6 +621,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -605,7 +644,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="1"/>
   <c:style val="2"/>
   <c:chart>
@@ -816,10 +855,6 @@
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:oneCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2287,7 +2322,50 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:14" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A5" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="G5" s="24">
+        <v>4</v>
+      </c>
+      <c r="H5" s="24">
+        <v>4</v>
+      </c>
+      <c r="I5" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="J5" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="K5" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="L5" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="M5" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
     <row r="6" spans="1:14" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:14" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:14" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -6295,6 +6373,7 @@
     <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <phoneticPr fontId="10" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C10" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
     <hyperlink ref="F10" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>

</xml_diff>